<commit_message>
chore: changed default password
</commit_message>
<xml_diff>
--- a/resources/users.xlsx
+++ b/resources/users.xlsx
@@ -31,12 +31,6 @@
     <t>HASH</t>
   </si>
   <si>
-    <t>$2b$12$163Xomqumv0L5RBnHHg.5.uZ5pdCXqYDNwOgxGN6zTqRzzoAhPvKy</t>
-  </si>
-  <si>
-    <t>8c6976e5b5410415bde908bd4dee15dfb167a9c873fc4bb8a81f6f2ab448a918</t>
-  </si>
-  <si>
     <t>USERNAME</t>
   </si>
   <si>
@@ -50,13 +44,19 @@
   </si>
   <si>
     <t>$2b$12$DBdcWOkawxYcsvDGsNtMruhWENMPv74euyAyZ1ScyCInRQaWMfQm6</t>
+  </si>
+  <si>
+    <t>$2b$12$QxPEm5z1OAJzc0SFHvqKNecF7nq4DkeciWCVAPcXZgkTE3NAlU8JS</t>
+  </si>
+  <si>
+    <t>6a1bbc448a668c31e0cfe425b018f299b0d9dcb666ebb5ec1819e276d5ec9550</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +65,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,12 +100,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -407,7 +418,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -421,7 +432,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -438,10 +449,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -452,10 +463,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -466,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: added two profiles - admin and editor
</commit_message>
<xml_diff>
--- a/resources/users.xlsx
+++ b/resources/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>PASSWORD</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>6a1bbc448a668c31e0cfe425b018f299b0d9dcb666ebb5ec1819e276d5ec9550</t>
+  </si>
+  <si>
+    <t>PROFILE</t>
+  </si>
+  <si>
+    <t>editor</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -427,10 +433,11 @@
     <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="22.42578125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -440,8 +447,11 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -454,8 +464,11 @@
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -468,8 +481,11 @@
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -481,6 +497,9 @@
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: change logins and passwords
</commit_message>
<xml_diff>
--- a/resources/users.xlsx
+++ b/resources/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>PASSWORD</t>
   </si>
@@ -22,30 +22,12 @@
     <t>admin</t>
   </si>
   <si>
-    <t>fulano</t>
-  </si>
-  <si>
-    <t>beltrano</t>
-  </si>
-  <si>
     <t>HASH</t>
   </si>
   <si>
     <t>USERNAME</t>
   </si>
   <si>
-    <t>e7a90381498109efe5501ec479f31405f9ffde1ba403fd2e0a9921d4fdd037ee</t>
-  </si>
-  <si>
-    <t>42349e8b571738904cb8d649a3a14d5764a9df9bf2ccfbf456484eefa94462f4</t>
-  </si>
-  <si>
-    <t>$2b$12$/UBTfwnMP/54UjRv6cR6.Og.haFd8dFi6q0z5t77dCy7iQCndk2XG</t>
-  </si>
-  <si>
-    <t>$2b$12$DBdcWOkawxYcsvDGsNtMruhWENMPv74euyAyZ1ScyCInRQaWMfQm6</t>
-  </si>
-  <si>
     <t>$2b$12$QxPEm5z1OAJzc0SFHvqKNecF7nq4DkeciWCVAPcXZgkTE3NAlU8JS</t>
   </si>
   <si>
@@ -56,6 +38,18 @@
   </si>
   <si>
     <t>editor</t>
+  </si>
+  <si>
+    <t>$2b$12$v1uTTh7BSg4Y9IxSekCoXORKtLD1CCeoyLC6MeWuDWjBkCQQUuDfuP/54UjRv6cR6.Og.haFd8dFi6q0z5t77dCy7iQCndk2XG</t>
+  </si>
+  <si>
+    <t>$2b$12$e5xG2DT48B0fecxMI7Qhe..f1D47.vXuxvxCLlmHkePwuurFvf3nC</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>744f26fa641bc48221956243d43d6a3dfcf88776927f3a5cc397eb130d910630</t>
   </si>
 </sst>
 </file>
@@ -424,7 +418,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -433,22 +427,22 @@
     <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -459,12 +453,12 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -473,16 +467,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,16 +484,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: updated editor password
</commit_message>
<xml_diff>
--- a/resources/users.xlsx
+++ b/resources/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>PASSWORD</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>editor</t>
-  </si>
-  <si>
-    <t>$2b$12$v1uTTh7BSg4Y9IxSekCoXORKtLD1CCeoyLC6MeWuDWjBkCQQUuDfuP/54UjRv6cR6.Og.haFd8dFi6q0z5t77dCy7iQCndk2XG</t>
   </si>
   <si>
     <t>$2b$12$e5xG2DT48B0fecxMI7Qhe..f1D47.vXuxvxCLlmHkePwuurFvf3nC</t>
@@ -415,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -473,7 +470,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -484,17 +481,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>